<commit_message>
add stt and tts with updated app
</commit_message>
<xml_diff>
--- a/data/excel/henkel_inventory_dummy_data.xlsx
+++ b/data/excel/henkel_inventory_dummy_data.xlsx
@@ -3481,7 +3481,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -9587,7 +9587,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="3" t="s">
         <v>586</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="3" t="s">
         <v>591</v>
       </c>
@@ -9707,7 +9707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="3" t="s">
         <v>597</v>
       </c>
@@ -9767,7 +9767,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="3" t="s">
         <v>603</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="3" t="s">
         <v>609</v>
       </c>
@@ -9889,7 +9889,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="3" t="s">
         <v>614</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="3" t="s">
         <v>618</v>
       </c>
@@ -10007,7 +10007,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="3" t="s">
         <v>624</v>
       </c>
@@ -10069,7 +10069,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="3" t="s">
         <v>630</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
       <c r="A106" s="3" t="s">
         <v>636</v>
       </c>
@@ -10189,7 +10189,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
       <c r="A107" s="3" t="s">
         <v>641</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
       <c r="A108" s="3" t="s">
         <v>646</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
       <c r="A109" s="3" t="s">
         <v>650</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
       <c r="A110" s="3" t="s">
         <v>654</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
       <c r="A111" s="3" t="s">
         <v>659</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
       <c r="A112" s="3" t="s">
         <v>665</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
       <c r="A113" s="3" t="s">
         <v>672</v>
       </c>

</xml_diff>